<commit_message>
Corrected sperring errors for url
</commit_message>
<xml_diff>
--- a/Outline.xlsx
+++ b/Outline.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chiek\Desktop\Java\REST\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D648E083-95B1-4287-A514-54EF0E558998}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D37718F-4D0F-4B69-98C4-97AF30052E2D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14380" windowHeight="4090" xr2:uid="{7AEA7A7E-A247-442B-9FA1-9F54A281A0DE}"/>
   </bookViews>
@@ -247,18 +247,6 @@
     <t>userId;</t>
   </si>
   <si>
-    <t>ychieko</t>
-  </si>
-  <si>
-    <t>test1</t>
-  </si>
-  <si>
-    <t>test2</t>
-  </si>
-  <si>
-    <t>test3</t>
-  </si>
-  <si>
     <t>demo</t>
   </si>
   <si>
@@ -320,9 +308,6 @@
   </si>
   <si>
     <t>api/books/all</t>
-  </si>
-  <si>
-    <t>api/books/genru/{genru}</t>
   </si>
   <si>
     <t>api/books?book_id={bookId}</t>
@@ -420,13 +405,7 @@
     <t>Get book list (ALL)</t>
   </si>
   <si>
-    <t>Get book list by genru</t>
-  </si>
-  <si>
     <t>Get book details for each book</t>
-  </si>
-  <si>
-    <t>Get genru list</t>
   </si>
   <si>
     <t>Login</t>
@@ -562,13 +541,34 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">1. Users review a book list for each genru.
+      <t xml:space="preserve">1. Users review a book list for each genre.
 2. Users can add books to a shopping cart and buy them via Stripe payment.
 3. User can write a review for each book, and also edit/delete their reviews. 
 4. Users with 'ADMIN' role can delete any reviews. 
 5. User can create new user account.
  </t>
     </r>
+  </si>
+  <si>
+    <t>Get book list by genre</t>
+  </si>
+  <si>
+    <t>Get genre list</t>
+  </si>
+  <si>
+    <t>api/books/genre/{genre}</t>
+  </si>
+  <si>
+    <t>admin</t>
+  </si>
+  <si>
+    <t>user1</t>
+  </si>
+  <si>
+    <t>user2</t>
+  </si>
+  <si>
+    <t>user3</t>
   </si>
 </sst>
 </file>
@@ -1211,22 +1211,22 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>247650</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>31750</xdr:rowOff>
+      <xdr:colOff>596900</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>165100</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>101600</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>2787650</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="8" name="Picture 7">
+        <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C48CEB9B-7D30-4BE0-9709-CE96C7518206}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{09CA83E5-DADB-4199-8168-AB3104A4D23B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1249,8 +1249,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="247650" y="215900"/>
-          <a:ext cx="7232650" cy="4673600"/>
+          <a:off x="596900" y="171450"/>
+          <a:ext cx="5988050" cy="4972050"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1571,7 +1571,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71300177-1736-461D-A2DB-4DD245948F49}">
   <dimension ref="C2:N28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C16" sqref="C16:N28"/>
     </sheetView>
   </sheetViews>
@@ -1582,7 +1582,7 @@
   <sheetData>
     <row r="2" spans="3:14" ht="23.5" x14ac:dyDescent="0.55000000000000004">
       <c r="C2" s="28" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
     </row>
     <row r="3" spans="3:14" x14ac:dyDescent="0.35">
@@ -1649,7 +1649,7 @@
     </row>
     <row r="11" spans="3:14" x14ac:dyDescent="0.35">
       <c r="C11" s="70" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="D11" s="71"/>
       <c r="E11" s="71"/>
@@ -1658,7 +1658,7 @@
     </row>
     <row r="12" spans="3:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C12" s="73" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="D12" s="68"/>
       <c r="E12" s="68"/>
@@ -1686,7 +1686,7 @@
     </row>
     <row r="16" spans="3:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C16" s="55" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
       <c r="D16" s="56"/>
       <c r="E16" s="56"/>
@@ -1887,8 +1887,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{270C5208-4617-48BE-A76F-48EB58F4BA21}">
   <dimension ref="B14:F93"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="C103" sqref="C103"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2004,14 +2004,14 @@
     </row>
     <row r="38" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B38" s="17" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="C38" s="8"/>
       <c r="D38" s="11"/>
     </row>
     <row r="39" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B39" s="17" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="C39" s="8"/>
       <c r="D39" s="11"/>
@@ -2052,29 +2052,29 @@
     </row>
     <row r="43" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B43" s="10" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="C43" s="8" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="D43" s="11" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
     </row>
     <row r="44" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B44" s="10" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="C44" s="8" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="D44" s="11" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
     </row>
     <row r="45" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B45" s="22" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="C45" s="15"/>
       <c r="D45" s="16"/>
@@ -2094,18 +2094,18 @@
         <v>60</v>
       </c>
       <c r="D47" s="11" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
     </row>
     <row r="48" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B48" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="C48" s="8" t="s">
         <v>148</v>
       </c>
-      <c r="C48" s="8" t="s">
-        <v>155</v>
-      </c>
       <c r="D48" s="11" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
     </row>
     <row r="49" spans="2:4" x14ac:dyDescent="0.35">
@@ -2135,13 +2135,13 @@
     </row>
     <row r="52" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B52" s="10" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="C52" s="8" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="D52" s="11" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
     </row>
     <row r="53" spans="2:4" x14ac:dyDescent="0.35">
@@ -2291,7 +2291,7 @@
     </row>
     <row r="72" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B72" s="17" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="C72" s="8"/>
       <c r="D72" s="11"/>
@@ -2309,7 +2309,7 @@
     </row>
     <row r="74" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B74" s="17" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="C74" s="8"/>
       <c r="D74" s="11"/>
@@ -2327,7 +2327,7 @@
     </row>
     <row r="76" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B76" s="17" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="C76" s="8"/>
       <c r="D76" s="11"/>
@@ -2345,7 +2345,7 @@
     </row>
     <row r="78" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B78" s="17" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="C78" s="8"/>
       <c r="D78" s="11"/>
@@ -2363,7 +2363,7 @@
     </row>
     <row r="80" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B80" s="17" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="C80" s="8"/>
       <c r="D80" s="11"/>
@@ -2472,7 +2472,7 @@
   <dimension ref="A2:F16"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2486,7 +2486,7 @@
   <sheetData>
     <row r="2" spans="1:6" ht="66.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="36" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="B2" s="36" t="s">
         <v>57</v>
@@ -2495,21 +2495,21 @@
         <v>58</v>
       </c>
       <c r="D2" s="42" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="E2" s="37" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="3" spans="1:6" s="50" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="43" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="B3" s="43" t="s">
         <v>55</v>
       </c>
       <c r="C3" s="43" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="D3" s="43" t="s">
         <v>59</v>
@@ -2521,13 +2521,13 @@
     </row>
     <row r="4" spans="1:6" s="50" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A4" s="43" t="s">
-        <v>127</v>
+        <v>158</v>
       </c>
       <c r="B4" s="43" t="s">
         <v>55</v>
       </c>
       <c r="C4" s="43" t="s">
-        <v>97</v>
+        <v>160</v>
       </c>
       <c r="D4" s="43" t="s">
         <v>59</v>
@@ -2539,13 +2539,13 @@
     </row>
     <row r="5" spans="1:6" s="50" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A5" s="43" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="B5" s="43" t="s">
         <v>55</v>
       </c>
       <c r="C5" s="43" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="D5" s="43" t="s">
         <v>59</v>
@@ -2557,13 +2557,13 @@
     </row>
     <row r="6" spans="1:6" s="50" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A6" s="43" t="s">
-        <v>129</v>
+        <v>159</v>
       </c>
       <c r="B6" s="43" t="s">
         <v>55</v>
       </c>
       <c r="C6" s="43" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="D6" s="43" t="s">
         <v>59</v>
@@ -2575,16 +2575,16 @@
     </row>
     <row r="7" spans="1:6" s="50" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A7" s="43" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="B7" s="43" t="s">
         <v>55</v>
       </c>
       <c r="C7" s="43" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="D7" s="43" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="E7" s="43" t="s">
         <v>59</v>
@@ -2593,67 +2593,67 @@
     </row>
     <row r="8" spans="1:6" s="50" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A8" s="43" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="B8" s="43" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="C8" s="43" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="D8" s="43" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="E8" s="47" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="F8" s="51"/>
     </row>
     <row r="9" spans="1:6" s="50" customFormat="1" ht="58" x14ac:dyDescent="0.35">
       <c r="A9" s="43" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="B9" s="43" t="s">
         <v>56</v>
       </c>
       <c r="C9" s="43" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="D9" s="47" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="E9" s="47" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="F9" s="51"/>
     </row>
     <row r="10" spans="1:6" s="50" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A10" s="43" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="B10" s="43" t="s">
         <v>56</v>
       </c>
       <c r="C10" s="43" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="D10" s="47" t="s">
         <v>59</v>
       </c>
       <c r="E10" s="47" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="F10" s="51"/>
     </row>
     <row r="11" spans="1:6" s="50" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A11" s="47" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="B11" s="43" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="C11" s="47" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="D11" s="43" t="s">
         <v>59</v>
@@ -2663,16 +2663,16 @@
     </row>
     <row r="12" spans="1:6" s="50" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A12" s="43" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="B12" s="43" t="s">
         <v>55</v>
       </c>
       <c r="C12" s="43" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="D12" s="43" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="E12" s="43" t="s">
         <v>59</v>
@@ -2681,13 +2681,13 @@
     </row>
     <row r="13" spans="1:6" s="50" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A13" s="43" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="B13" s="43" t="s">
         <v>55</v>
       </c>
       <c r="C13" s="43" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="D13" s="43" t="s">
         <v>59</v>
@@ -2699,16 +2699,16 @@
     </row>
     <row r="14" spans="1:6" s="50" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A14" s="48" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="B14" s="43" t="s">
         <v>56</v>
       </c>
       <c r="C14" s="48" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="D14" s="43" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="E14" s="43" t="s">
         <v>59</v>
@@ -2741,97 +2741,97 @@
   <sheetData>
     <row r="2" spans="2:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B2" s="44" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="C2" s="44" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="D2" s="44" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
     </row>
     <row r="3" spans="2:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B3" s="45" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="C3" s="46" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="D3" s="46" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
     </row>
     <row r="4" spans="2:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B4" s="45" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="C4" s="45" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="D4" s="45" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
     </row>
     <row r="5" spans="2:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B5" s="45" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="C5" s="46" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="D5" s="45"/>
     </row>
     <row r="6" spans="2:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B6" s="45" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="C6" s="45" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="D6" s="45"/>
     </row>
     <row r="7" spans="2:4" ht="31" x14ac:dyDescent="0.35">
       <c r="B7" s="45" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="C7" s="46" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="D7" s="46" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
     </row>
     <row r="8" spans="2:4" ht="46.5" x14ac:dyDescent="0.35">
       <c r="B8" s="45" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="C8" s="46" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="D8" s="46" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
     </row>
     <row r="9" spans="2:4" ht="31" x14ac:dyDescent="0.35">
       <c r="B9" s="45" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="C9" s="46" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="D9" s="46" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
     </row>
     <row r="10" spans="2:4" ht="31" x14ac:dyDescent="0.35">
       <c r="B10" s="45" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="C10" s="46" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="D10" s="46" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
     </row>
   </sheetData>
@@ -2845,7 +2845,7 @@
   <dimension ref="B2:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2859,92 +2859,92 @@
   <sheetData>
     <row r="2" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B2" s="31" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B3" s="39" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C3" s="39" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="D3" s="39" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="E3" s="39" t="s">
         <v>24</v>
       </c>
       <c r="F3" s="39" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B4" s="40" t="s">
+        <v>161</v>
+      </c>
+      <c r="C4" s="40" t="s">
         <v>72</v>
       </c>
-      <c r="C4" s="40" t="s">
+      <c r="D4" s="40" t="s">
         <v>76</v>
       </c>
-      <c r="D4" s="40" t="s">
-        <v>80</v>
-      </c>
       <c r="E4" s="40" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="F4" s="40" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B5" s="40" t="s">
-        <v>73</v>
+        <v>162</v>
       </c>
       <c r="C5" s="40" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="D5" s="40" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="E5" s="40" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="F5" s="40" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B6" s="40" t="s">
-        <v>74</v>
+        <v>163</v>
       </c>
       <c r="C6" s="40" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="D6" s="40" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="E6" s="40" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="F6" s="40" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B7" s="40" t="s">
-        <v>75</v>
+        <v>164</v>
       </c>
       <c r="C7" s="40" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="D7" s="40" t="s">
+        <v>82</v>
+      </c>
+      <c r="E7" s="40" t="s">
+        <v>83</v>
+      </c>
+      <c r="F7" s="40" t="s">
         <v>86</v>
-      </c>
-      <c r="E7" s="40" t="s">
-        <v>87</v>
-      </c>
-      <c r="F7" s="40" t="s">
-        <v>90</v>
       </c>
     </row>
   </sheetData>

</xml_diff>